<commit_message>
Criação das tabelas base e de domínio
</commit_message>
<xml_diff>
--- a/ChatGPT/ChatGPTDOC.xlsx
+++ b/ChatGPT/ChatGPTDOC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IGOR\IGOR\IgorAyelloBorges\PROJETOS\FinancialMarketSimulatorRealData\ChatGPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216D95B4-4DD6-47B9-B6DB-F286F8437E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8AC8AF-91B2-48ED-8920-77AB8111BEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{94286A15-74E0-4448-8809-569685BF6ECD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Pergunta</t>
   </si>
@@ -424,6 +424,140 @@
 👉 [http://localhost:8000/docs](http://localhost:8000/docs)
 ---
 Isso deve resolver o erro de importação! Se precisar de mais alguma coisa, me avise.</t>
+  </si>
+  <si>
+    <t>Criar tabela SegmentoClassificacao</t>
+  </si>
+  <si>
+    <t>Criar tabela Segmento</t>
+  </si>
+  <si>
+    <t>Criar tabela Subsetor</t>
+  </si>
+  <si>
+    <t>Criar tabela SetorEconomico</t>
+  </si>
+  <si>
+    <t>Criar tabela Empresa</t>
+  </si>
+  <si>
+    <t>Preciso gerar um script para criar uma tabela no SQL Server onde deverá constar a primary key identity ID, a sigla e o descritivo.</t>
+  </si>
+  <si>
+    <t>Aqui está o **script SQL** para criar a tabela no **SQL Server** conforme sua necessidade:  
+### **Criação da Tabela**  
+```sql
+CREATE TABLE dbo.TabelaBDR (
+    ID INT IDENTITY(1,1) PRIMARY KEY,  -- Chave primária autoincrementada
+    Sigla VARCHAR(10) NOT NULL,        -- Sigla extraída dos parênteses
+    Descritivo VARCHAR(255) NOT NULL   -- Texto após os parênteses
+);
+```
+### **Explicação do Código**
+1. **`ID`** → Chave primária autoincrementada (`IDENTITY(1,1)`)
+2. **`Sigla`** → Campo para armazenar a sigla (texto dentro dos parênteses)
+3. **`Descritivo`** → Campo para armazenar o descritivo (texto após os parênteses)
+Caso precise popular a tabela com dados extraídos de uma planilha ou fonte de dados externa, me avise que posso ajudar com o script para inserção e transformação dos dados! 🚀</t>
+  </si>
+  <si>
+    <t>Preciso gerar um script para criar uma tabela no SQL Server com o nome "Setor Econômico" onde deverá constar a primary key identity ID e o descritivo.</t>
+  </si>
+  <si>
+    <t>Aqui está o **script SQL** para criar a tabela `Setor Econômico` no **SQL Server**:  
+### **Criação da Tabela**  
+```sql
+CREATE TABLE dbo.[Setor Econômico] (
+    ID INT IDENTITY(1,1) PRIMARY KEY,  -- Chave primária autoincrementada
+    Descritivo VARCHAR(255) NOT NULL   -- Nome do setor econômico
+);
+```
+### **Explicação do Código**
+1. **`ID`** → Chave primária autoincrementada (`IDENTITY(1,1)`)
+2. **`Descritivo`** → Campo para armazenar o nome do setor econômico (obrigatório com `NOT NULL`)
+&gt; **Observação:**  
+&gt; Como o nome da tabela contém espaço (`Setor Econômico`), usei **colchetes** (`[]`) para evitar erros. Se preferir, pode usar um nome sem espaço, como `Setor_Economico`.
+Caso precise popular a tabela com valores iniciais, me avise! 🚀</t>
+  </si>
+  <si>
+    <t>Preciso gerar um script para criar uma tabela no SQL Server com o nome "Subsetor" onde deverá constar a primary key identity ID e o descritivo.</t>
+  </si>
+  <si>
+    <t>Preciso gerar um script para criar uma tabela no SQL Server com o nome "Segmento" onde deverá constar a primary key identity ID e o descritivo.</t>
+  </si>
+  <si>
+    <t>Aqui está o **script SQL** para criar a tabela `Segmento` no **SQL Server**:  
+### **Criação da Tabela**  
+```sql
+CREATE TABLE dbo.Segmento (
+    ID INT IDENTITY(1,1) PRIMARY KEY,  -- Chave primária autoincrementada
+    Descritivo VARCHAR(255) NOT NULL   -- Nome do segmento
+);
+```
+### **Explicação do Código**
+1. **`ID`** → Chave primária autoincrementada (`IDENTITY(1,1)`)
+2. **`Descritivo`** → Campo para armazenar o nome do segmento (**obrigatório com `NOT NULL`**)  
+Caso precise relacionar essa tabela com **Setor Econômico** ou **Subsetor**, me avise para adicionar as chaves estrangeiras (`FOREIGN KEY`). 🚀</t>
+  </si>
+  <si>
+    <t>Aqui está o **script SQL** para criar a tabela `Subsetor` no **SQL Server**:  
+### **Criação da Tabela**  
+```sql
+CREATE TABLE dbo.Subsetor (
+    ID INT IDENTITY(1,1) PRIMARY KEY,  -- Chave primária autoincrementada
+    Descritivo VARCHAR(255) NOT NULL   -- Nome do subsetor
+);
+```
+### **Explicação do Código**
+1. **`ID`** → Chave primária autoincrementada (`IDENTITY(1,1)`)
+2. **`Descritivo`** → Campo para armazenar o nome do subsetor (**obrigatório com `NOT NULL`**)  
+Caso precise relacionar essa tabela com a tabela **Setor Econômico**, me avise para adicionar a chave estrangeira (`FOREIGN KEY`). 🚀</t>
+  </si>
+  <si>
+    <t>Preciso gerar um script para criar uma tabela no SQL Server com o nome "Empresa" onde deverá constar a primary key identity ID, Nome, código (sigla) fazendo chave estrangeira para as seguintes 
+tabelas dbo.SegmentoClassificacao (NÃO obrigatória), SetorEconomico (obrigatória), Subsetor (obrigatória) e Segmento (obrigatória).</t>
+  </si>
+  <si>
+    <t>Aqui está o **script SQL** para criar a tabela `Empresa` no **SQL Server**, com as chaves estrangeiras conforme sua especificação:  
+### **Criação da Tabela `Empresa`**  
+```sql
+CREATE TABLE dbo.Empresa (
+    ID INT IDENTITY(1,1) PRIMARY KEY,  -- Chave primária autoincrementada
+    Nome VARCHAR(255) NOT NULL,         -- Nome da empresa
+    Codigo VARCHAR(50) NOT NULL,        -- Código/Sigla da empresa
+    -- Chaves estrangeiras
+    SegmentoClassificacaoID INT NULL,   -- FK opcional (NÃO obrigatória)
+    SetorEconomicoID INT NOT NULL,      -- FK obrigatória
+    SubsetorID INT NOT NULL,            -- FK obrigatória
+    SegmentoID INT NOT NULL,            -- FK obrigatória
+    -- Definição das chaves estrangeiras
+    CONSTRAINT FK_Empresa_SegmentoClassificacao FOREIGN KEY (SegmentoClassificacaoID) 
+        REFERENCES dbo.SegmentoClassificacao(ID),
+    CONSTRAINT FK_Empresa_SetorEconomico FOREIGN KEY (SetorEconomicoID) 
+        REFERENCES dbo.SetorEconomico(ID),
+    CONSTRAINT FK_Empresa_Subsetor FOREIGN KEY (SubsetorID) 
+        REFERENCES dbo.Subsetor(ID),
+    CONSTRAINT FK_Empresa_Segmento FOREIGN KEY (SegmentoID) 
+        REFERENCES dbo.Segmento(ID)
+);
+```
+---
+### **Explicação do Código**
+1. **`ID`** → Chave primária autoincrementada (`IDENTITY(1,1)`)
+2. **`Nome`** → Nome da empresa (**Obrigatório com `NOT NULL`**)
+3. **`Codigo`** → Código ou sigla da empresa (**Obrigatório com `NOT NULL`**)
+4. **`SegmentoClassificacaoID`** → Chave estrangeira **opcional** (`NULL permitido`)
+5. **`SetorEconomicoID`**, **`SubsetorID`**, **`SegmentoID`** → Chaves estrangeiras **obrigatórias** (`NOT NULL`)
+### **Relacionamentos**
+| Tabela                  | Obrigatoriedade | Chave Estrangeira |
+|-------------------------|----------------|-------------------|
+| SegmentoClassificacao   | ❌ (Opcional)   | `SegmentoClassificacaoID` |
+| SetorEconomico         | ✅ (Obrigatória) | `SetorEconomicoID` |
+| Subsetor               | ✅ (Obrigatória) | `SubsetorID` |
+| Segmento               | ✅ (Obrigatória) | `SegmentoID` |
+---
+### **O que fazer agora?**
+✔️ Se as tabelas referenciadas (`SegmentoClassificacao`, `SetorEconomico`, `Subsetor`, `Segmento`) ainda **não existirem**, crie-as antes de rodar este script.  
+✔️ Caso precise adicionar **índices** ou **constraints adicionais**, me avise. 🚀</t>
   </si>
 </sst>
 </file>
@@ -801,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C306EA0C-B462-426C-9093-F405642008FF}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,7 +1019,7 @@
         <v>0.74722222222222223</v>
       </c>
       <c r="G3" s="6">
-        <f t="shared" ref="G3:G5" si="0">F3-E3</f>
+        <f t="shared" ref="G3:G10" si="0">F3-E3</f>
         <v>1.2499999999999956E-2</v>
       </c>
     </row>
@@ -926,6 +1060,111 @@
       <c r="G5" s="2">
         <f t="shared" si="0"/>
         <v>3.4722222222222099E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.90902777777777777</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.91041666666666665</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>1.388888888888884E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.91111111111111109</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.91249999999999998</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>1.388888888888884E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="345" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.91319444444444442</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.9145833333333333</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>1.388888888888884E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="360" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.9145833333333333</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.91805555555555551</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>3.4722222222222099E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.91805555555555551</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.92291666666666672</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>4.8611111111112049E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>